<commit_message>
meta data 에 primary key 정보 추가
</commit_message>
<xml_diff>
--- a/sample_excel.xlsx
+++ b/sample_excel.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16828"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -13,7 +13,6 @@
   </bookViews>
   <sheets>
     <sheet name="sample" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,16 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>no:I</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>name:T</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>height:N</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -116,6 +111,14 @@
   </si>
   <si>
     <t>sim</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no:I:PK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name:T:PK</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -338,13 +341,10 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -375,29 +375,29 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -716,13 +716,13 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.25" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="8.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.125" customWidth="1"/>
     <col min="5" max="5" width="1.625" customWidth="1"/>
@@ -732,176 +732,176 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="16"/>
+      <c r="F1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="15"/>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="16"/>
+      <c r="I1" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="15"/>
-      <c r="I1" s="5" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="13">
+        <v>1</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="6">
+        <v>185.5</v>
+      </c>
+      <c r="D4" s="7">
+        <v>25</v>
+      </c>
+      <c r="F4" s="13"/>
+      <c r="G4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="6">
+        <v>193.8</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="G5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6">
+        <v>170</v>
+      </c>
+      <c r="D6" s="17">
+        <v>27</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
+        <v>4</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6">
+        <v>180</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="13"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="11">
+        <v>5</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="10" t="s">
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="F8" s="6">
+        <v>2</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="I8" s="13"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I9" s="13"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I10" s="6">
         <v>8</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="12">
-        <v>1</v>
-      </c>
-      <c r="G3" s="7" t="s">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I11" s="6">
         <v>9</v>
       </c>
-      <c r="I3" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
-        <v>1</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="7">
-        <v>185.5</v>
-      </c>
-      <c r="D4" s="8">
-        <v>25</v>
-      </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="7">
-        <v>2</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="7">
-        <v>193.8</v>
-      </c>
-      <c r="D5" s="8">
-        <v>0</v>
-      </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="7">
-        <v>3</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="7">
-        <v>170</v>
-      </c>
-      <c r="D6" s="16">
-        <v>27</v>
-      </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="7">
-        <v>4</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="7">
-        <v>180</v>
-      </c>
-      <c r="D7" s="17"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="12"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="18">
-        <v>5</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="F8" s="7">
-        <v>2</v>
-      </c>
-      <c r="G8" s="7"/>
-      <c r="I8" s="12"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I9" s="12"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I10" s="7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I11" s="7">
-        <v>9</v>
-      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I12" s="7">
+      <c r="I12" s="6">
         <v>10</v>
       </c>
     </row>
@@ -917,74 +917,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>